<commit_message>
All Done! For real this time!
</commit_message>
<xml_diff>
--- a/Sprint4/Lab 4 Analysis.xlsx
+++ b/Sprint4/Lab 4 Analysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2484D28-AB85-4A55-88A0-662071022B9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EFBA8ADE-E7B1-49F7-838C-60E1DF28FA19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -215,6 +215,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,7 +841,1678 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lab 4 Algorithm vs Lab 3 Algorithm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Efficiency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0200000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7200000000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>3.4299999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.47E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4049-4656-9860-2EDCD3B43B75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic Programming</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.1699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8399999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.63E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.7999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>8.2900000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4049-4656-9860-2EDCD3B43B75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Genetic Algorithm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$J$3:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.0400000000000004E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6199999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>1.03E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9100000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5099999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8900000000000001E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4049-4656-9860-2EDCD3B43B75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tabu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$K$3:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.2999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2599999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2799999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2299999999999995E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4600000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9899999999999999E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4049-4656-9860-2EDCD3B43B75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="700009056"/>
+        <c:axId val="700009384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="700009056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.51954046369203855"/>
+              <c:y val="0.77277704870224551"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="700009384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="700009384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Runtime</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="700009056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lab 4 Algorithm vs Lab 3 Algorithm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Efficiency (Logarithmic)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0200000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7200000000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>3.4299999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.47E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-214F-4F4D-B207-D8C45778D100}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic Programming</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.1699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8399999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.63E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.7999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>8.2900000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-214F-4F4D-B207-D8C45778D100}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Genetic Algorithm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$J$3:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.0400000000000004E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6199999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>1.03E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9100000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5099999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8900000000000001E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-214F-4F4D-B207-D8C45778D100}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DATA!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tabu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$K$3:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.2999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2599999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2799999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2299999999999995E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4600000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9899999999999999E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-214F-4F4D-B207-D8C45778D100}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="700009056"/>
+        <c:axId val="700009384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="700009056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.51954046369203855"/>
+              <c:y val="0.77277704870224551"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="700009384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="700009384"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Runtime</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="700009056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1393,6 +3068,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1428,6 +4135,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09368C19-6394-42E2-A224-EF081E5E6343}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A28FF3B9-3E6D-42DB-B4DC-35B8C436C238}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1735,8 +4518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,10 +4590,10 @@
         <v>4</v>
       </c>
       <c r="H3" s="5">
-        <v>2.4300000000000001E-5</v>
+        <v>1.0200000000000001E-5</v>
       </c>
       <c r="I3" s="18">
-        <v>1.26E-5</v>
+        <v>2.1699999999999999E-5</v>
       </c>
       <c r="J3" s="20">
         <v>7.0400000000000004E-5</v>
@@ -1839,10 +4622,10 @@
         <v>5</v>
       </c>
       <c r="H4" s="7">
-        <v>4.5200000000000001E-5</v>
+        <v>1.5699999999999999E-5</v>
       </c>
       <c r="I4" s="19">
-        <v>2.2099999999999998E-5</v>
+        <v>1.8600000000000001E-5</v>
       </c>
       <c r="J4" s="21">
         <v>4.6199999999999998E-5</v>
@@ -1867,10 +4650,10 @@
         <v>6</v>
       </c>
       <c r="H5" s="5">
-        <v>5.6999999999999998E-4</v>
+        <v>7.7200000000000006E-5</v>
       </c>
       <c r="I5" s="18">
-        <v>6.2399999999999999E-4</v>
+        <v>2.8399999999999999E-5</v>
       </c>
       <c r="J5" s="4">
         <v>1.03E-4</v>
@@ -1896,11 +4679,11 @@
       <c r="G6" s="6">
         <v>7</v>
       </c>
-      <c r="H6" s="7">
-        <v>3.16E-3</v>
-      </c>
-      <c r="I6" s="19">
-        <v>1.39E-3</v>
+      <c r="H6" s="22">
+        <v>3.4299999999999999E-4</v>
+      </c>
+      <c r="I6" s="23">
+        <v>1.63E-4</v>
       </c>
       <c r="J6" s="21">
         <v>3.9100000000000002E-5</v>
@@ -1928,11 +4711,11 @@
       <c r="G7" s="4">
         <v>8</v>
       </c>
-      <c r="H7" s="5">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="I7" s="18">
-        <v>7.2700000000000004E-3</v>
+      <c r="H7" s="24">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="I7" s="25">
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="J7" s="20">
         <v>4.5099999999999998E-5</v>
@@ -1956,11 +4739,11 @@
       <c r="G8" s="6">
         <v>9</v>
       </c>
-      <c r="H8" s="7">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="I8" s="19">
-        <v>9.1399999999999995E-2</v>
+      <c r="H8" s="22">
+        <v>2.47E-2</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0.01</v>
       </c>
       <c r="J8" s="21">
         <v>2.8600000000000001E-5</v>
@@ -1984,11 +4767,11 @@
       <c r="G9" s="4">
         <v>10</v>
       </c>
-      <c r="H9" s="5">
-        <v>1.17</v>
-      </c>
-      <c r="I9" s="18">
-        <v>0.55600000000000005</v>
+      <c r="H9" s="24">
+        <v>0.19</v>
+      </c>
+      <c r="I9" s="25">
+        <v>8.2900000000000001E-2</v>
       </c>
       <c r="J9" s="20">
         <v>2.8900000000000001E-5</v>
@@ -2248,7 +5031,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixing Report and Analyis
</commit_message>
<xml_diff>
--- a/Sprint4/Lab 4 Analysis.xlsx
+++ b/Sprint4/Lab 4 Analysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EFBA8ADE-E7B1-49F7-838C-60E1DF28FA19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53C1B7D5-0A46-4D2E-B73B-2E5F542061DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Number of Nodes</t>
   </si>
@@ -4516,10 +4516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4529,8 +4529,7 @@
     <col min="3" max="4" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -4977,6 +4976,15 @@
       <c r="D25" s="5">
         <v>1.5699999999999999E-4</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
@@ -4987,6 +4995,15 @@
       <c r="D26" s="7">
         <v>2.9300000000000002E-4</v>
       </c>
+      <c r="G26" s="4">
+        <v>4</v>
+      </c>
+      <c r="H26" s="18">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="I26" s="20">
+        <v>7.0400000000000004E-5</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
@@ -4997,6 +5014,15 @@
       <c r="D27" s="5">
         <v>5.7899999999999998E-4</v>
       </c>
+      <c r="G27" s="6">
+        <v>5</v>
+      </c>
+      <c r="H27" s="19">
+        <v>1.8600000000000001E-5</v>
+      </c>
+      <c r="I27" s="21">
+        <v>4.6199999999999998E-5</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="8"/>
@@ -5006,6 +5032,15 @@
       <c r="D28" s="7">
         <v>7.8399999999999997E-4</v>
       </c>
+      <c r="G28" s="4">
+        <v>6</v>
+      </c>
+      <c r="H28" s="18">
+        <v>2.8399999999999999E-5</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1.03E-4</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C29" s="4">
@@ -5013,6 +5048,136 @@
       </c>
       <c r="D29" s="5">
         <v>1.07E-3</v>
+      </c>
+      <c r="G29" s="6">
+        <v>7</v>
+      </c>
+      <c r="H29" s="23">
+        <v>1.63E-4</v>
+      </c>
+      <c r="I29" s="21">
+        <v>3.9100000000000002E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G30" s="4">
+        <v>8</v>
+      </c>
+      <c r="H30" s="25">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="I30" s="20">
+        <v>4.5099999999999998E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G31" s="6">
+        <v>9</v>
+      </c>
+      <c r="H31" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="I31" s="21">
+        <v>2.8600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G32" s="4">
+        <v>10</v>
+      </c>
+      <c r="H32" s="25">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="I32" s="20">
+        <v>2.8900000000000001E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G35" s="4">
+        <v>4</v>
+      </c>
+      <c r="H35" s="18">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="I35" s="5">
+        <v>8.2999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G36" s="6">
+        <v>5</v>
+      </c>
+      <c r="H36" s="19">
+        <v>1.8600000000000001E-5</v>
+      </c>
+      <c r="I36" s="7">
+        <v>2.2599999999999999E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G37" s="4">
+        <v>6</v>
+      </c>
+      <c r="H37" s="18">
+        <v>2.8399999999999999E-5</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1.2799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G38" s="6">
+        <v>7</v>
+      </c>
+      <c r="H38" s="23">
+        <v>1.63E-4</v>
+      </c>
+      <c r="I38" s="7">
+        <v>8.2299999999999995E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G39" s="4">
+        <v>8</v>
+      </c>
+      <c r="H39" s="25">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="I39" s="5">
+        <v>2.4600000000000002E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G40" s="6">
+        <v>9</v>
+      </c>
+      <c r="H40" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="I40" s="7">
+        <v>5.24E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G41" s="4">
+        <v>10</v>
+      </c>
+      <c r="H41" s="25">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="I41" s="5">
+        <v>5.9899999999999999E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>